<commit_message>
Regresion lineal en v-x
</commit_message>
<xml_diff>
--- a/Graphs.xlsx
+++ b/Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuent\OneDrive\Documents\2019\Física 2\UpdatedRepo\SunRotation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33675C3-ED8F-4C48-BE2A-CF904F66E7D5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A511391E-01B1-4E0C-831A-37AE22C17EDD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Velocidad</t>
   </si>
@@ -116,12 +116,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -154,14 +161,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="17" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -196,6 +206,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Velocidad - Tiempo</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -277,8 +312,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="4"/>
+            <c:trendlineType val="linear"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -667,8 +701,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Velocidad - Altura</a:t>
+              <a:t>Velocidad Angular - Distancia</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> del Ecuador</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -754,21 +793,27 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="poly"/>
-            <c:order val="4"/>
+            <c:order val="2"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.43118678915135605"/>
-                  <c:y val="-0.39324438611840185"/>
+                  <c:x val="-0.43396456692913388"/>
+                  <c:y val="-0.25015851717474008"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                  <a:miter lim="800000"/>
                 </a:ln>
                 <a:effectLst/>
               </c:spPr>
@@ -779,10 +824,7 @@
                   <a:pPr>
                     <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
+                        <a:schemeClr val="dk1"/>
                       </a:solidFill>
                       <a:latin typeface="+mn-lt"/>
                       <a:ea typeface="+mn-ea"/>
@@ -904,6 +946,9 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0.2455</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.30120000000000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0.21029999999999999</c:v>
@@ -1122,6 +1167,478 @@
     <c:title>
       <c:tx>
         <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Velocidad Angular-Altura</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-GT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$D$93</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Velocidad</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.15408486439195102"/>
+                  <c:y val="-0.28522511101528281"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:prstDash val="solid"/>
+                  <a:miter lim="800000"/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-GT"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$C$94:$C$110</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1019</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1174</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.67249999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.52629999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$D$94:$D$110</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.20630000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1928</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.217</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17949999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2107</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.21099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.15509999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1731</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1925</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.2286</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.24560000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.20469999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.22600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.2455</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.21029999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1217-4DD9-936A-1FACACECD60D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="745690792"/>
+        <c:axId val="745691120"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="745690792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-GT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="745691120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="745691120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-GT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="745690792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-GT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
@@ -1500,7 +2017,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -2117,6 +2634,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3666,6 +4223,522 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4250,6 +5323,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>594845</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>131857</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5166845</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>73586</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C41ED4A6-B954-41D2-8374-5F6F8223EEDD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4940,10 +6049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="D88" zoomScale="152" workbookViewId="0">
+      <selection activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -5536,7 +6645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="3:4">
+    <row r="49" spans="3:6">
       <c r="C49">
         <f>AVERAGE([1]Hoja1!$C$3:$C$8)</f>
         <v>-0.1325692645787647</v>
@@ -5545,7 +6654,7 @@
         <v>0.20630000000000001</v>
       </c>
     </row>
-    <row r="50" spans="3:4">
+    <row r="50" spans="3:6">
       <c r="C50">
         <f>AVERAGE([2]Hoja1!$C$2:$C$9)</f>
         <v>0.11189639641799043</v>
@@ -5554,7 +6663,7 @@
         <v>0.1928</v>
       </c>
     </row>
-    <row r="51" spans="3:4">
+    <row r="51" spans="3:6">
       <c r="C51">
         <f>AVERAGE([3]Hoja1!$C$2:$C$9)</f>
         <v>2.8577304662659314E-2</v>
@@ -5563,7 +6672,7 @@
         <v>0.217</v>
       </c>
     </row>
-    <row r="52" spans="3:4">
+    <row r="52" spans="3:6">
       <c r="C52">
         <f>AVERAGE([4]Hoja1!$C$2:$C$7)</f>
         <v>0.42664100155335749</v>
@@ -5572,7 +6681,7 @@
         <v>0.17949999999999999</v>
       </c>
     </row>
-    <row r="53" spans="3:4">
+    <row r="53" spans="3:6">
       <c r="C53">
         <f>AVERAGE([5]Hoja1!$C$2:$C$9)</f>
         <v>0.10199594656224928</v>
@@ -5581,7 +6690,7 @@
         <v>0.2107</v>
       </c>
     </row>
-    <row r="54" spans="3:4">
+    <row r="54" spans="3:6">
       <c r="C54">
         <f>AVERAGE([6]sample22006!$C$11:$C$14)</f>
         <v>0.11742329555710174</v>
@@ -5590,7 +6699,7 @@
         <v>0.21099999999999999</v>
       </c>
     </row>
-    <row r="55" spans="3:4">
+    <row r="55" spans="3:6">
       <c r="C55">
         <f>AVERAGE([7]Hoja1!$C$2:$C$4)</f>
         <v>-0.67250923101842408</v>
@@ -5599,7 +6708,7 @@
         <v>0.15509999999999999</v>
       </c>
     </row>
-    <row r="56" spans="3:4">
+    <row r="56" spans="3:6">
       <c r="C56">
         <f>AVERAGE([8]Hoja1!$C$2:$C$4)</f>
         <v>-0.52630099920186602</v>
@@ -5608,7 +6717,7 @@
         <v>0.1731</v>
       </c>
     </row>
-    <row r="57" spans="3:4">
+    <row r="57" spans="3:6">
       <c r="C57">
         <v>0.18</v>
       </c>
@@ -5616,7 +6725,7 @@
         <v>0.1925</v>
       </c>
     </row>
-    <row r="58" spans="3:4">
+    <row r="58" spans="3:6">
       <c r="C58">
         <v>-0.3</v>
       </c>
@@ -5624,7 +6733,7 @@
         <v>0.27110000000000001</v>
       </c>
     </row>
-    <row r="59" spans="3:4">
+    <row r="59" spans="3:6">
       <c r="C59">
         <v>-0.06</v>
       </c>
@@ -5632,7 +6741,7 @@
         <v>0.2286</v>
       </c>
     </row>
-    <row r="60" spans="3:4">
+    <row r="60" spans="3:6">
       <c r="C60">
         <v>-0.11</v>
       </c>
@@ -5640,7 +6749,7 @@
         <v>0.24560000000000001</v>
       </c>
     </row>
-    <row r="61" spans="3:4">
+    <row r="61" spans="3:6">
       <c r="C61">
         <v>0.1</v>
       </c>
@@ -5648,7 +6757,7 @@
         <v>0.20469999999999999</v>
       </c>
     </row>
-    <row r="62" spans="3:4">
+    <row r="62" spans="3:6">
       <c r="C62">
         <v>-0.24</v>
       </c>
@@ -5656,7 +6765,7 @@
         <v>0.22600000000000001</v>
       </c>
     </row>
-    <row r="63" spans="3:4">
+    <row r="63" spans="3:6">
       <c r="C63">
         <v>0.12</v>
       </c>
@@ -5664,9 +6773,15 @@
         <v>0.2455</v>
       </c>
     </row>
-    <row r="64" spans="3:4">
+    <row r="64" spans="3:6">
       <c r="C64">
         <v>-0.6</v>
+      </c>
+      <c r="D64">
+        <v>0.30120000000000002</v>
+      </c>
+      <c r="F64">
+        <v>0.27110000000000001</v>
       </c>
     </row>
     <row r="65" spans="3:6">
@@ -5678,6 +6793,296 @@
       </c>
       <c r="F65">
         <v>0.30120000000000002</v>
+      </c>
+    </row>
+    <row r="73" spans="3:6">
+      <c r="C73" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="3:6">
+      <c r="C74">
+        <f>AVERAGE([1]Hoja1!$C$3:$C$8)</f>
+        <v>-0.1325692645787647</v>
+      </c>
+      <c r="D74">
+        <v>0.20630000000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="3:6">
+      <c r="C75">
+        <f>AVERAGE([2]Hoja1!$C$2:$C$9)</f>
+        <v>0.11189639641799043</v>
+      </c>
+      <c r="D75">
+        <v>0.1928</v>
+      </c>
+    </row>
+    <row r="76" spans="3:6">
+      <c r="C76">
+        <f>AVERAGE([3]Hoja1!$C$2:$C$9)</f>
+        <v>2.8577304662659314E-2</v>
+      </c>
+      <c r="D76">
+        <v>0.217</v>
+      </c>
+    </row>
+    <row r="77" spans="3:6">
+      <c r="C77">
+        <f>AVERAGE([4]Hoja1!$C$2:$C$7)</f>
+        <v>0.42664100155335749</v>
+      </c>
+      <c r="D77">
+        <v>0.17949999999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="3:6">
+      <c r="C78">
+        <f>AVERAGE([5]Hoja1!$C$2:$C$9)</f>
+        <v>0.10199594656224928</v>
+      </c>
+      <c r="D78">
+        <v>0.2107</v>
+      </c>
+    </row>
+    <row r="79" spans="3:6">
+      <c r="C79">
+        <f>AVERAGE([6]sample22006!$C$11:$C$14)</f>
+        <v>0.11742329555710174</v>
+      </c>
+      <c r="D79">
+        <v>0.21099999999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="3:6">
+      <c r="C80">
+        <f>AVERAGE([7]Hoja1!$C$2:$C$4)</f>
+        <v>-0.67250923101842408</v>
+      </c>
+      <c r="D80">
+        <v>0.15509999999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4">
+      <c r="C81">
+        <f>AVERAGE([8]Hoja1!$C$2:$C$4)</f>
+        <v>-0.52630099920186602</v>
+      </c>
+      <c r="D81">
+        <v>0.1731</v>
+      </c>
+    </row>
+    <row r="82" spans="3:4">
+      <c r="C82">
+        <v>0.18</v>
+      </c>
+      <c r="D82">
+        <v>0.1925</v>
+      </c>
+    </row>
+    <row r="83" spans="3:4">
+      <c r="C83">
+        <v>-0.3</v>
+      </c>
+      <c r="D83">
+        <v>0.27110000000000001</v>
+      </c>
+    </row>
+    <row r="84" spans="3:4">
+      <c r="C84">
+        <v>-0.06</v>
+      </c>
+      <c r="D84">
+        <v>0.2286</v>
+      </c>
+    </row>
+    <row r="85" spans="3:4">
+      <c r="C85">
+        <v>-0.11</v>
+      </c>
+      <c r="D85">
+        <v>0.24560000000000001</v>
+      </c>
+    </row>
+    <row r="86" spans="3:4">
+      <c r="C86">
+        <v>0.1</v>
+      </c>
+      <c r="D86">
+        <v>0.20469999999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="3:4">
+      <c r="C87">
+        <v>-0.24</v>
+      </c>
+      <c r="D87">
+        <v>0.22600000000000001</v>
+      </c>
+    </row>
+    <row r="88" spans="3:4">
+      <c r="C88">
+        <v>0.12</v>
+      </c>
+      <c r="D88">
+        <v>0.2455</v>
+      </c>
+    </row>
+    <row r="89" spans="3:4">
+      <c r="C89">
+        <v>-0.6</v>
+      </c>
+      <c r="D89">
+        <v>0.30120000000000002</v>
+      </c>
+    </row>
+    <row r="90" spans="3:4">
+      <c r="C90">
+        <v>-0.12</v>
+      </c>
+      <c r="D90">
+        <v>0.21029999999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="3:4">
+      <c r="C93" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="3:4">
+      <c r="C94">
+        <v>0.13</v>
+      </c>
+      <c r="D94">
+        <v>0.20630000000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="3:4">
+      <c r="C95">
+        <v>0.11</v>
+      </c>
+      <c r="D95">
+        <v>0.1928</v>
+      </c>
+    </row>
+    <row r="96" spans="3:4">
+      <c r="C96">
+        <v>0.02</v>
+      </c>
+      <c r="D96">
+        <v>0.217</v>
+      </c>
+    </row>
+    <row r="97" spans="3:4">
+      <c r="C97">
+        <v>0.42</v>
+      </c>
+      <c r="D97">
+        <v>0.17949999999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="3:4">
+      <c r="C98">
+        <v>0.1019</v>
+      </c>
+      <c r="D98">
+        <v>0.2107</v>
+      </c>
+    </row>
+    <row r="99" spans="3:4">
+      <c r="C99">
+        <v>0.1174</v>
+      </c>
+      <c r="D99">
+        <v>0.21099999999999999</v>
+      </c>
+    </row>
+    <row r="100" spans="3:4">
+      <c r="C100">
+        <v>0.67249999999999999</v>
+      </c>
+      <c r="D100">
+        <v>0.15509999999999999</v>
+      </c>
+    </row>
+    <row r="101" spans="3:4">
+      <c r="C101">
+        <v>0.52629999999999999</v>
+      </c>
+      <c r="D101">
+        <v>0.1731</v>
+      </c>
+    </row>
+    <row r="102" spans="3:4">
+      <c r="C102">
+        <v>0.18</v>
+      </c>
+      <c r="D102">
+        <v>0.1925</v>
+      </c>
+    </row>
+    <row r="103" spans="3:4">
+      <c r="C103">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="104" spans="3:4">
+      <c r="C104">
+        <v>0.06</v>
+      </c>
+      <c r="D104">
+        <v>0.2286</v>
+      </c>
+    </row>
+    <row r="105" spans="3:4">
+      <c r="C105">
+        <v>0.11</v>
+      </c>
+      <c r="D105">
+        <v>0.24560000000000001</v>
+      </c>
+    </row>
+    <row r="106" spans="3:4">
+      <c r="C106">
+        <v>0.1</v>
+      </c>
+      <c r="D106">
+        <v>0.20469999999999999</v>
+      </c>
+    </row>
+    <row r="107" spans="3:4">
+      <c r="C107">
+        <v>0.24</v>
+      </c>
+      <c r="D107">
+        <v>0.22600000000000001</v>
+      </c>
+    </row>
+    <row r="108" spans="3:4">
+      <c r="C108">
+        <v>0.12</v>
+      </c>
+      <c r="D108">
+        <v>0.2455</v>
+      </c>
+    </row>
+    <row r="109" spans="3:4">
+      <c r="C109">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="110" spans="3:4">
+      <c r="C110">
+        <v>0.12</v>
+      </c>
+      <c r="D110">
+        <v>0.21029999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>